<commit_message>
Update new test version
</commit_message>
<xml_diff>
--- a/HW1/Q2/Q2_Summary.xlsx
+++ b/HW1/Q2/Q2_Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cetun\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cetun\Documents\WorkSpace\CS402-Product\HW1\Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9B095F-F6CA-4660-9DE1-E39495641DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA0E49A-8D25-4984-BD8D-0DC279D6B60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E7323BC5-FFAE-4E9B-8DC5-E3F707645C64}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="25155" windowHeight="11295" xr2:uid="{E7323BC5-FFAE-4E9B-8DC5-E3F707645C64}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -457,32 +457,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,9 +502,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -542,7 +542,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -648,7 +648,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -790,7 +790,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -801,7 +801,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,81 +821,81 @@
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="21"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="19"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="17">
         <v>2.6</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18">
+      <c r="C3" s="17"/>
+      <c r="D3" s="17">
         <v>3.2</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18">
+      <c r="E3" s="17"/>
+      <c r="F3" s="17">
         <v>2.6</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18">
+      <c r="G3" s="17"/>
+      <c r="H3" s="17">
         <v>3.2</v>
       </c>
-      <c r="I3" s="19"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="19">
         <v>1279</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20">
         <v>359.99</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="14">
+      <c r="E4" s="20"/>
+      <c r="F4" s="19">
         <v>1279</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15">
+      <c r="G4" s="20"/>
+      <c r="H4" s="20">
         <v>359.99</v>
       </c>
-      <c r="I4" s="15"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -960,10 +960,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="1">
-        <v>2.9610579000000001</v>
+        <v>2.6991195000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>3.0206840000000001</v>
+        <v>3.4457911999999999</v>
       </c>
       <c r="D7" s="1">
         <v>4.0672262000000003</v>
@@ -972,10 +972,10 @@
         <v>3.9129228999999999</v>
       </c>
       <c r="F7" s="1">
-        <v>2.2810193999999999</v>
+        <v>2.7715443999999998</v>
       </c>
       <c r="G7" s="1">
-        <v>2.3852356000000001</v>
+        <v>3.1346018999999998</v>
       </c>
       <c r="H7" s="1">
         <v>4.1863923999999999</v>
@@ -989,10 +989,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="1">
-        <v>2.4880374999999999</v>
+        <v>3.2145093</v>
       </c>
       <c r="C8" s="1">
-        <v>3.1734734000000002</v>
+        <v>3.2764133000000002</v>
       </c>
       <c r="D8" s="1">
         <v>3.5418351000000001</v>
@@ -1001,10 +1001,10 @@
         <v>3.7724345000000001</v>
       </c>
       <c r="F8" s="1">
-        <v>2.3330109000000001</v>
+        <v>2.747382</v>
       </c>
       <c r="G8" s="1">
-        <v>2.6344243000000001</v>
+        <v>3.0668829</v>
       </c>
       <c r="H8" s="1">
         <v>3.4363733999999999</v>
@@ -1018,10 +1018,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="1">
-        <v>2.3643736999999998</v>
+        <v>2.8794694000000001</v>
       </c>
       <c r="C9" s="1">
-        <v>4.1115576000000003</v>
+        <v>3.8868437</v>
       </c>
       <c r="D9" s="1">
         <v>5.3317934999999999</v>
@@ -1030,10 +1030,10 @@
         <v>4.1079534999999998</v>
       </c>
       <c r="F9" s="1">
-        <v>2.3286229999999999</v>
+        <v>2.8575379000000001</v>
       </c>
       <c r="G9" s="1">
-        <v>2.4017279999999999</v>
+        <v>3.0284472</v>
       </c>
       <c r="H9" s="1">
         <v>4.5663342</v>
@@ -1047,10 +1047,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="1">
-        <v>2.2511055999999998</v>
+        <v>3.1354462999999999</v>
       </c>
       <c r="C10" s="1">
-        <v>3.0032228000000001</v>
+        <v>3.6504748</v>
       </c>
       <c r="D10" s="1">
         <v>3.8857556999999998</v>
@@ -1059,10 +1059,10 @@
         <v>3.8070664000000001</v>
       </c>
       <c r="F10" s="1">
-        <v>2.7860255999999999</v>
+        <v>2.9364864000000002</v>
       </c>
       <c r="G10" s="1">
-        <v>2.7575166000000002</v>
+        <v>2.8996875000000002</v>
       </c>
       <c r="H10" s="1">
         <v>4.4247402999999998</v>
@@ -1076,10 +1076,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="1">
-        <v>2.2146058000000002</v>
+        <v>2.7922465999999999</v>
       </c>
       <c r="C11" s="1">
-        <v>2.8190667999999999</v>
+        <v>3.0659391999999999</v>
       </c>
       <c r="D11" s="1">
         <v>5.4365863000000001</v>
@@ -1088,10 +1088,10 @@
         <v>3.6301944000000002</v>
       </c>
       <c r="F11" s="1">
-        <v>2.4545466</v>
+        <v>2.8128964000000001</v>
       </c>
       <c r="G11" s="1">
-        <v>2.7321955999999998</v>
+        <v>2.9729133000000001</v>
       </c>
       <c r="H11" s="1">
         <v>4.4716646999999998</v>
@@ -1105,10 +1105,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="1">
-        <v>2.2453416000000002</v>
+        <v>2.7839860000000001</v>
       </c>
       <c r="C12" s="1">
-        <v>3.2760699999999998</v>
+        <v>3.1860879</v>
       </c>
       <c r="D12" s="1">
         <v>3.7203571000000002</v>
@@ -1117,10 +1117,10 @@
         <v>3.8003721000000001</v>
       </c>
       <c r="F12" s="1">
-        <v>2.3940920000000001</v>
+        <v>2.4901371000000001</v>
       </c>
       <c r="G12" s="1">
-        <v>2.6714093999999999</v>
+        <v>2.7965848000000002</v>
       </c>
       <c r="H12" s="1">
         <v>3.7602381999999999</v>
@@ -1134,10 +1134,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="1">
-        <v>2.3450479</v>
+        <v>2.6809129</v>
       </c>
       <c r="C13" s="1">
-        <v>3.3012655999999998</v>
+        <v>3.5040548</v>
       </c>
       <c r="D13" s="1">
         <v>5.1066675999999998</v>
@@ -1146,10 +1146,10 @@
         <v>3.9416134999999999</v>
       </c>
       <c r="F13" s="1">
-        <v>2.6068050999999999</v>
+        <v>2.5793282999999998</v>
       </c>
       <c r="G13" s="1">
-        <v>2.7651338000000001</v>
+        <v>2.7896592999999998</v>
       </c>
       <c r="H13" s="1">
         <v>4.4781978999999996</v>
@@ -1163,10 +1163,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="1">
-        <v>2.3841160000000001</v>
+        <v>2.7007859000000001</v>
       </c>
       <c r="C14" s="1">
-        <v>2.7827362</v>
+        <v>3.3613854000000001</v>
       </c>
       <c r="D14" s="1">
         <v>4.1231416999999997</v>
@@ -1175,10 +1175,10 @@
         <v>3.8668824000000002</v>
       </c>
       <c r="F14" s="1">
-        <v>2.6092572000000001</v>
+        <v>2.8467715999999998</v>
       </c>
       <c r="G14" s="1">
-        <v>2.6187388999999999</v>
+        <v>2.7968076000000002</v>
       </c>
       <c r="H14" s="1">
         <v>3.0595086</v>
@@ -1192,10 +1192,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="1">
-        <v>2.3358595000000002</v>
+        <v>2.9032792999999999</v>
       </c>
       <c r="C15" s="1">
-        <v>2.6360556000000002</v>
+        <v>3.7371998999999998</v>
       </c>
       <c r="D15" s="1">
         <v>4.9113227999999998</v>
@@ -1204,10 +1204,10 @@
         <v>15.005610000000001</v>
       </c>
       <c r="F15" s="1">
-        <v>2.5247039</v>
+        <v>2.7628591999999998</v>
       </c>
       <c r="G15" s="1">
-        <v>2.7843065</v>
+        <v>2.6985579999999998</v>
       </c>
       <c r="H15" s="1">
         <v>4.4660342000000002</v>
@@ -1221,10 +1221,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="1">
-        <v>2.6309721000000001</v>
+        <v>2.9310341000000002</v>
       </c>
       <c r="C16" s="1">
-        <v>2.6276255000000002</v>
+        <v>3.2000755999999999</v>
       </c>
       <c r="D16" s="1">
         <v>3.6327937000000001</v>
@@ -1233,10 +1233,10 @@
         <v>6.7947685</v>
       </c>
       <c r="F16" s="1">
-        <v>2.4480145000000002</v>
+        <v>2.6775926000000001</v>
       </c>
       <c r="G16" s="1">
-        <v>2.5959514000000001</v>
+        <v>2.9112787999999998</v>
       </c>
       <c r="H16" s="1">
         <v>3.6182234000000002</v>
@@ -1251,11 +1251,11 @@
       </c>
       <c r="B17" s="7">
         <f t="shared" ref="B17:I17" si="0">AVERAGE(B7:B16)</f>
-        <v>2.42205176</v>
+        <v>2.8720789299999998</v>
       </c>
       <c r="C17" s="7">
         <f t="shared" si="0"/>
-        <v>3.0751757499999997</v>
+        <v>3.4314265800000001</v>
       </c>
       <c r="D17" s="7">
         <f t="shared" si="0"/>
@@ -1267,11 +1267,11 @@
       </c>
       <c r="F17" s="7">
         <f t="shared" si="0"/>
-        <v>2.4766098200000002</v>
+        <v>2.74825359</v>
       </c>
       <c r="G17" s="7">
         <f t="shared" si="0"/>
-        <v>2.6346640100000003</v>
+        <v>2.9095421299999997</v>
       </c>
       <c r="H17" s="7">
         <f t="shared" si="0"/>
@@ -1288,11 +1288,11 @@
       </c>
       <c r="B18" s="9">
         <f t="shared" ref="B18:I18" si="1">1/B17</f>
-        <v>0.41287309235703534</v>
+        <v>0.34817984615764025</v>
       </c>
       <c r="C18" s="9">
         <f t="shared" si="1"/>
-        <v>0.325184666274765</v>
+        <v>0.29142398261658276</v>
       </c>
       <c r="D18" s="9">
         <f t="shared" si="1"/>
@@ -1304,11 +1304,11 @@
       </c>
       <c r="F18" s="9">
         <f t="shared" si="1"/>
-        <v>0.40377777392484049</v>
+        <v>0.36386744063163401</v>
       </c>
       <c r="G18" s="9">
         <f t="shared" si="1"/>
-        <v>0.3795550385948453</v>
+        <v>0.34369669017303422</v>
       </c>
       <c r="H18" s="9">
         <f t="shared" si="1"/>
@@ -1325,110 +1325,108 @@
       </c>
       <c r="B19" s="11">
         <f>D17/B17</f>
-        <v>1.8066285957489203</v>
+        <v>1.5235472550192071</v>
       </c>
       <c r="C19" s="11">
         <f>E17/C17</f>
-        <v>1.7117661714131303</v>
+        <v>1.5340505464056877</v>
       </c>
       <c r="D19" s="11">
         <f>B17/D17</f>
-        <v>0.55351719902643282</v>
+        <v>0.65636296918627135</v>
       </c>
       <c r="E19" s="11">
         <f>C17/E17</f>
-        <v>0.58419193970544514</v>
+        <v>0.65186900284545435</v>
       </c>
       <c r="F19" s="11">
         <f>H17/F17</f>
-        <v>1.6339960769436019</v>
+        <v>1.4724881083481094</v>
       </c>
       <c r="G19" s="11">
         <f>I17/G17</f>
-        <v>1.0616864311286509</v>
+        <v>0.96138392400593997</v>
       </c>
       <c r="H19" s="11">
         <f>F17/H17</f>
-        <v>0.61199657337642155</v>
+        <v>0.67912263218331614</v>
       </c>
       <c r="I19" s="12">
         <f>G17/I17</f>
-        <v>0.94189769284036751</v>
+        <v>1.0401671746633256</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="17">
         <f>B3/D3</f>
         <v>0.8125</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18">
+      <c r="C20" s="17"/>
+      <c r="D20" s="17">
         <f>D3/B3</f>
         <v>1.2307692307692308</v>
       </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18">
+      <c r="E20" s="17"/>
+      <c r="F20" s="17">
         <f>F3/H3</f>
         <v>0.8125</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18">
+      <c r="G20" s="17"/>
+      <c r="H20" s="17">
         <f>H3/F3</f>
         <v>1.2307692307692308</v>
       </c>
-      <c r="I20" s="18"/>
+      <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="21">
         <f>D4/B4</f>
         <v>0.28146207974980453</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="16">
+      <c r="C21" s="22"/>
+      <c r="D21" s="21">
         <f>B4/D4</f>
         <v>3.5528764687907994</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="16">
+      <c r="E21" s="22"/>
+      <c r="F21" s="21">
         <f>H4/F4</f>
         <v>0.28146207974980453</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="16">
+      <c r="G21" s="22"/>
+      <c r="H21" s="21">
         <f>F4/H4</f>
         <v>3.5528764687907994</v>
       </c>
-      <c r="I21" s="17"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="14" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
@@ -1441,10 +1439,12 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>